<commit_message>
thay vì phải dùng tới tham số --use-api ||| Dùng cột useApiOrPrompt để quyết định việc sử dụng API hay Prompt
Thêm 1 cột như này trong file input

	Note	STT	roleA_prompt	roleB_prompt	initialConversationHistory	maxTurns	useApiOrPrompt
		1	You are Cuong. You are AI Assistant	You are Minh. You are AI Assistant	"[
    {""role"": ""roleA"", ""content"": ""What is your name?""}
]"	2	prompt
		2	You are Cuong. You are AI Assistant	You are Minh. You are AI Assistant	"[
    {""role"": ""roleB"", ""content"": ""What is your name?""}
]"	2	prompt
		2	You are Cuong. You are AI Assistant	You are Minh. You are AI Assistant	"[
    {""role"": ""roleA"", ""content"": ""sẵn sàng""}
]"	2	api

----
thay vì phải dùng tới tham số --use-api
</commit_message>
<xml_diff>
--- a/6_TuningWith2Prompting/src/result.xlsx
+++ b/6_TuningWith2Prompting/src/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
   <si>
     <t>Role</t>
   </si>
@@ -22,56 +22,85 @@
     <t>Content</t>
   </si>
   <si>
-    <t>Response_Time</t>
-  </si>
-  <si>
-    <t>RoleA_Prompt</t>
-  </si>
-  <si>
-    <t>RoleB_Prompt</t>
+    <t>Response Time</t>
+  </si>
+  <si>
+    <t>RoleA Prompt</t>
+  </si>
+  <si>
+    <t>RoleB Prompt</t>
+  </si>
+  <si>
+    <t>useApiOrPrompt</t>
+  </si>
+  <si>
+    <t>roleA</t>
   </si>
   <si>
     <t>roleB</t>
   </si>
   <si>
-    <t>roleA</t>
-  </si>
-  <si>
     <t>Separator</t>
   </si>
   <si>
+    <t>What is your name?</t>
+  </si>
+  <si>
+    <t>My name is Minh, and I'm here to assist you! How can I help you today?</t>
+  </si>
+  <si>
+    <t>Hello, Minh! How can I assist you today?</t>
+  </si>
+  <si>
+    <t>Hello! I'm here to assist you, so feel free to ask me anything or let me know what you need help with today!</t>
+  </si>
+  <si>
+    <t>Thank you, Minh! If you have any questions or need assistance with something specific, just let me know. I'm here to help!</t>
+  </si>
+  <si>
+    <t>-------------------</t>
+  </si>
+  <si>
+    <t>My name is Cuong, and I'm here to assist you! How can I help you today?</t>
+  </si>
+  <si>
+    <t>Hi Cuong! I'm here to help you with any questions or tasks you have. What can I assist you with today?</t>
+  </si>
+  <si>
+    <t>Hi! It seems like you might have mixed up our roles a bit. I'm here to assist you! If you have any questions or tasks you need help with, feel free to ask. What can I do for you today?</t>
+  </si>
+  <si>
+    <t>Thank you for the clarification, Cuong! I appreciate your willingness to assist. If you have any questions or topics you'd like to discuss, feel free to let me know. How can I help you today?</t>
+  </si>
+  <si>
     <t>Chào cậu! Hôm nay chúng ta sẽ học về chủ đề đồ ăn nhé! Các món ăn yêu thích của cậu là gì nào?</t>
   </si>
   <si>
     <t>Chào bạn! Mặc dù mình không có sở thích cá nhân, nhưng mình có thể chia sẻ về nhiều món ăn phổ biến và được yêu thích. Một số món ăn nổi tiếng có thể kể đến như phở, bánh mì, sushi, pizza, và pasta. Bạn có món ăn nào yêu thích không? Hãy cùng thảo luận về nó nhé!</t>
   </si>
   <si>
-    <t>Wow, cậu biết nhiều món ăn ngon quá! Hôm nay, tớ sẽ chọn món phở để học từ vựng nhé! Phở là một món ăn rất nổi tiếng ở Việt Nam. Trong tiếng Anh, phở được gọi là "noodle soup". Cậu có thể nói "noodle soup" không?</t>
-  </si>
-  <si>
-    <t>Chắc chắn rồi! "Noodle soup" là cách gọi tiếng Anh cho phở. Đây là một món ăn rất đặc trưng của Việt Nam, thường được làm từ nước dùng thơm ngon, bánh phở và các loại thịt như bò hoặc gà, kèm theo rau thơm và gia vị. Bạn muốn tìm hiểu thêm về các thành phần của phở hay cách chế biến không?</t>
-  </si>
-  <si>
-    <t>Tuyệt vời! Cậu đã nói rất đúng về phở! Giờ tớ sẽ giới thiệu từ vựng tiếp theo nhé! Từ tiếp theo là "beef". Trong tiếng Việt, "beef" có nghĩa là thịt bò. Cậu có thể nói "beef" không?</t>
-  </si>
-  <si>
-    <t>-------------------</t>
-  </si>
-  <si>
-    <t>Wow, cậu biết nhiều món ăn ngon quá! Hôm nay, tớ muốn nói về món "fried chicken" (gà rán) nhé! Cậu có biết gà rán không?</t>
-  </si>
-  <si>
-    <t>Có chứ! Gà rán là một món ăn rất phổ biến và được yêu thích ở nhiều nơi trên thế giới. Món ăn này thường được chế biến bằng cách ướp gà với gia vị, sau đó lăn qua bột và chiên ngập dầu cho đến khi vàng giòn. Gà rán có thể được ăn kèm với nhiều loại sốt khác nhau, như sốt BBQ, sốt mật ong, hoặc sốt cay.
-Ngoài ra, gà rán cũng thường được phục vụ với các món ăn phụ như khoai tây chiên, salad, hoặc bánh mì. Bạn có thích gà rán không? Có món gà rán nào đặc biệt mà bạn thích không?</t>
-  </si>
-  <si>
-    <t>Tớ cũng rất thích gà rán! Giờ chúng ta sẽ học từ "fried chicken" nhé! Cậu hãy lặp lại sau tớ: "fried chicken".</t>
+    <t>Wow, cậu biết nhiều món ăn ngon quá! Hôm nay, tớ muốn nói về món "bánh mì" nhé! Trong tiếng Anh, "bánh mì" là "bread". Cậu có thể nói "bread" không?</t>
+  </si>
+  <si>
+    <t>Đúng rồi, "bánh mì" trong tiếng Anh là "bread". Tuy nhiên, khi nói về món bánh mì Việt Nam, người ta thường dùng từ "Vietnamese sandwich" hoặc "bánh mì" để chỉ riêng món ăn này. Bánh mì Việt Nam rất đặc biệt với nhiều loại nhân khác nhau như thịt, chả, rau sống và nước sốt. Bạn có thích ăn bánh mì không? Nếu có, bạn thích loại nhân nào nhất?</t>
+  </si>
+  <si>
+    <t>Cậu nói rất đúng! Bánh mì Việt Nam thật sự rất ngon! Tớ cũng thích bánh mì! Bây giờ, chúng ta sẽ học một từ khác nhé! Từ tiếp theo là "thịt". Trong tiếng Anh, "thịt" là "meat". Cậu có thể nói "meat" không?</t>
   </si>
   <si>
     <t>You are Cuong. You are AI Assistant</t>
   </si>
   <si>
+    <t>You are Minh. You are AI Assistant</t>
+  </si>
+  <si>
     <t>Using API</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>api</t>
   </si>
 </sst>
 </file>
@@ -429,13 +458,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,196 +480,340 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1.475976228713989</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>0.1173186302185059</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>2.072214365005493</v>
+        <v>0.8429925441741943</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>0.8691504001617432</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>2.555711030960083</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>1.8143310546875</v>
+        <v>1.158419847488403</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>0.1075222492218018</v>
+        <v>1.09621787071228</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>4.605872392654419</v>
+        <v>0.9802405834197998</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>1.955087661743164</v>
+        <v>1.546533584594727</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
       <c r="C12">
-        <v>2.913470983505249</v>
+        <v>1.285999298095703</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>0.1378581523895264</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>2.117332458496094</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>2.278918981552124</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>1.989442348480225</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>1.980495691299438</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[đã fix cứng:   "max_tokens": 1024,   "temperature": 0.0,   "top_p": 1,] CÓ VẺ VẪN CHƯA ĐỦ ĐỂ CỐ ĐỊNH KẾT QUẢ CÁC LẦN CHẠY --- LẦN TRƯỚC KHI TEST luồng ở v1, v2 mình cũng đã để ý việc này. CÁCH MÌNH ĐỀ XUẤT CHÍNH LÀ SET FULL CÁC THAM SỐ MODEL THÔI
```
[bot 24] bài Agent. (Mặc dù trong sheet đã được fix cứng: temperature=0, ...).
Khi test với cùng 1 start_message và user_first_message => Output vẫn trả ra đang khác nhau trong 2 lần chạy, nguyên nhân do đâu anh nhỉ, (theo lý thuyết fix cứng là nó ko chạy được kết quả). ??

{
  "max_tokens": 1024,
  "temperature": 0.0,
  "top_p": 1,
  "model": "gpt-4o-mini",
  "stream": false
}

Để kết quả cố định em nghĩ là sau mình fix cứng thêm full các tham số cho dễ testing ạ.
        temperature=0,
        max_completion_tokens=2048,
        top_p=1,
        frequency_penalty=0,
        presence_penalty=0
---
anh @Đinh Hùng, anh @Minh Hoang Duc .
```
</commit_message>
<xml_diff>
--- a/6_TuningWith2Prompting/src/result.xlsx
+++ b/6_TuningWith2Prompting/src/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Role</t>
   </si>
@@ -43,61 +43,37 @@
     <t>Separator</t>
   </si>
   <si>
-    <t>What is your name?</t>
-  </si>
-  <si>
-    <t>My name is Minh, and I'm here to assist you! How can I help you today?</t>
-  </si>
-  <si>
-    <t>Hello, Minh! How can I assist you today?</t>
-  </si>
-  <si>
-    <t>Hello! I'm here to assist you, so feel free to ask me anything or let me know what you need help with today!</t>
-  </si>
-  <si>
-    <t>Thank you, Minh! If you have any questions or need assistance with something specific, just let me know. I'm here to help!</t>
+    <t>sẵn sàng</t>
+  </si>
+  <si>
+    <t>Chào cậu! Hôm nay chúng ta sẽ học về chủ đề đồ ăn nhé! Các món ăn yêu thích của cậu là gì nào?</t>
+  </si>
+  <si>
+    <t>Chào bạn! Mặc dù mình không ăn uống như con người, nhưng mình có thể chia sẻ về nhiều món ăn thú vị. Một số món ăn phổ biến mà nhiều người yêu thích bao gồm:
+1. **Phở** - Món ăn truyền thống của Việt Nam với nước dùng thơm ngon, bánh phở mềm và thịt bò hoặc gà.
+2. **Sushi** - Món ăn Nhật Bản với cơm cuộn và các loại hải sản tươi sống.
+3. **Pizza** - Món ăn Ý với đế bánh mì nướng, sốt cà chua, phô mai và nhiều loại topping khác nhau.
+4. **Tacos** - Món ăn Mexico với bánh tortilla và các loại nhân như thịt, rau và sốt.
+5. **Curry** - Món ăn Ấn Độ với nước sốt gia vị và thường đi kèm với cơm hoặc bánh naan.
+Bạn có món ăn nào yêu thích không?</t>
+  </si>
+  <si>
+    <t>Wow, cậu biết nhiều món ăn ngon quá! Hôm nay, chúng ta sẽ học một số từ vựng liên quan đến đồ ăn nhé! Cậu có thích món nào trong số đó không? Chúng ta có thể bắt đầu với "phở" nhé! Trong tiếng Anh, "phở" là "noodle soup". Cậu có thể nói "noodle soup" không?</t>
+  </si>
+  <si>
+    <t>Chắc chắn rồi! "Noodle soup" là cách dịch tiếng Anh cho món "phở". Món ăn này rất đặc trưng với nước dùng thơm ngon và bánh phở mềm. Nếu bạn muốn, chúng ta có thể tiếp tục học thêm từ vựng liên quan đến "phở" hoặc các món ăn khác! Bạn có muốn tìm hiểu thêm về các thành phần trong phở không?</t>
+  </si>
+  <si>
+    <t>Tuyệt vời! Cậu đã nói đúng rồi! Giờ chúng ta sẽ học thêm một từ vựng khác nhé! Một thành phần quan trọng trong phở là "thịt bò". Trong tiếng Anh, "thịt bò" là "beef". Cậu có thể nói "beef" không?</t>
   </si>
   <si>
     <t>-------------------</t>
   </si>
   <si>
-    <t>My name is Cuong, and I'm here to assist you! How can I help you today?</t>
-  </si>
-  <si>
-    <t>Hi Cuong! I'm here to help you with any questions or tasks you have. What can I assist you with today?</t>
-  </si>
-  <si>
-    <t>Hi! It seems like you might have mixed up our roles a bit. I'm here to assist you! If you have any questions or tasks you need help with, feel free to ask. What can I do for you today?</t>
-  </si>
-  <si>
-    <t>Thank you for the clarification, Cuong! I appreciate your willingness to assist. If you have any questions or topics you'd like to discuss, feel free to let me know. How can I help you today?</t>
-  </si>
-  <si>
-    <t>Chào cậu! Hôm nay chúng ta sẽ học về chủ đề đồ ăn nhé! Các món ăn yêu thích của cậu là gì nào?</t>
-  </si>
-  <si>
-    <t>Chào bạn! Mặc dù mình không có sở thích cá nhân, nhưng mình có thể chia sẻ về nhiều món ăn phổ biến và được yêu thích. Một số món ăn nổi tiếng có thể kể đến như phở, bánh mì, sushi, pizza, và pasta. Bạn có món ăn nào yêu thích không? Hãy cùng thảo luận về nó nhé!</t>
-  </si>
-  <si>
-    <t>Wow, cậu biết nhiều món ăn ngon quá! Hôm nay, tớ muốn nói về món "bánh mì" nhé! Trong tiếng Anh, "bánh mì" là "bread". Cậu có thể nói "bread" không?</t>
-  </si>
-  <si>
-    <t>Đúng rồi, "bánh mì" trong tiếng Anh là "bread". Tuy nhiên, khi nói về món bánh mì Việt Nam, người ta thường dùng từ "Vietnamese sandwich" hoặc "bánh mì" để chỉ riêng món ăn này. Bánh mì Việt Nam rất đặc biệt với nhiều loại nhân khác nhau như thịt, chả, rau sống và nước sốt. Bạn có thích ăn bánh mì không? Nếu có, bạn thích loại nhân nào nhất?</t>
-  </si>
-  <si>
-    <t>Cậu nói rất đúng! Bánh mì Việt Nam thật sự rất ngon! Tớ cũng thích bánh mì! Bây giờ, chúng ta sẽ học một từ khác nhé! Từ tiếp theo là "thịt". Trong tiếng Anh, "thịt" là "meat". Cậu có thể nói "meat" không?</t>
-  </si>
-  <si>
     <t>You are Cuong. You are AI Assistant</t>
   </si>
   <si>
-    <t>You are Minh. You are AI Assistant</t>
-  </si>
-  <si>
     <t>Using API</t>
-  </si>
-  <si>
-    <t>prompt</t>
   </si>
   <si>
     <t>api</t>
@@ -458,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,13 +471,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -512,16 +488,16 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1.475976228713989</v>
+        <v>0.1227195262908936</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -532,16 +508,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0.8429925441741943</v>
+        <v>3.274816513061523</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -552,16 +528,16 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>0.8691504001617432</v>
+        <v>3.696239948272705</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -572,248 +548,46 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>1.158419847488403</v>
+        <v>1.971581935882568</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2.313379049301147</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>1.09621787071228</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
-        <v>0.9802405834197998</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>1.546533584594727</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>1.285999298095703</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>0.1378581523895264</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>2.117332458496094</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16">
-        <v>2.278918981552124</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17">
-        <v>1.989442348480225</v>
-      </c>
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <v>1.980495691299438</v>
-      </c>
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
         <v>0</v>
       </c>
     </row>

</xml_diff>